<commit_message>
Update Requirements and Use Cases.xlsx
</commit_message>
<xml_diff>
--- a/Documentation/Requirements and Use Cases.xlsx
+++ b/Documentation/Requirements and Use Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Braden\Projects\Unity\Pirate-Game\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C3A8478-8650-40BE-BB88-05F84239981D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3BE748-C6CE-490C-8F10-9C43BDAC00C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -655,16 +655,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -674,21 +666,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -708,13 +721,13 @@
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -758,20 +771,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{61C093FC-2F58-483C-BE9C-75B7BBC36BE1}" name="Table3" displayName="Table3" ref="A3:K17" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{61C093FC-2F58-483C-BE9C-75B7BBC36BE1}" name="Table3" displayName="Table3" ref="A3:K17" totalsRowShown="0" dataDxfId="11">
   <autoFilter ref="A3:K17" xr:uid="{61C093FC-2F58-483C-BE9C-75B7BBC36BE1}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{30E8F1A6-7CD2-4EF3-8E6F-56959CD646AA}" name="Tag" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{F52A7F49-E465-4FE1-A760-58DB1FE2B1E9}" name="Name" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{8016E8F8-D705-42C8-AF9A-6C7CA7489481}" name="Actor" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{C506213D-542B-439C-90B7-55E41A8352C1}" name="Use Case" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{43904210-5515-49C8-A716-7ACF4CF13F1B}" name="Preconditions" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{5788F87F-5C95-48B0-AE11-B7A563EB5D41}" name="Sequence" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{6EE0D9D4-73F2-4979-A2FB-22CE3D30A8EC}" name="Postconditions" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{A583119B-6CA1-4322-9550-F866C6A1BDE7}" name="Progress" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{B9E0B555-60B0-4A0A-8F62-7BE46FAD7372}" name="Number" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{DDF11260-8EDD-4F2D-9888-7E56F16A435E}" name="Fulfills" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{8A3D7912-315A-4E14-8D33-7075DED51DEB}" name="Required" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{30E8F1A6-7CD2-4EF3-8E6F-56959CD646AA}" name="Tag" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{F52A7F49-E465-4FE1-A760-58DB1FE2B1E9}" name="Name" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{8016E8F8-D705-42C8-AF9A-6C7CA7489481}" name="Actor" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{C506213D-542B-439C-90B7-55E41A8352C1}" name="Use Case" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{43904210-5515-49C8-A716-7ACF4CF13F1B}" name="Preconditions" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{5788F87F-5C95-48B0-AE11-B7A563EB5D41}" name="Sequence" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{6EE0D9D4-73F2-4979-A2FB-22CE3D30A8EC}" name="Postconditions" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{A583119B-6CA1-4322-9550-F866C6A1BDE7}" name="Progress" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{B9E0B555-60B0-4A0A-8F62-7BE46FAD7372}" name="Number" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{DDF11260-8EDD-4F2D-9888-7E56F16A435E}" name="Fulfills" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{8A3D7912-315A-4E14-8D33-7075DED51DEB}" name="Required" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1042,57 +1055,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.08984375" customWidth="1"/>
-    <col min="18" max="18" width="4.7265625" customWidth="1"/>
-    <col min="19" max="19" width="5" customWidth="1"/>
-    <col min="20" max="20" width="4.81640625" customWidth="1"/>
+    <col min="7" max="7" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="20" width="4.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="G1" s="3" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="G1" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1107,43 +1108,44 @@
       <c r="D2" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="8"/>
+      <c r="H2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="T2" s="9" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1154,25 +1156,25 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11" t="s">
+      <c r="H3" s="12"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13" t="s">
         <v>133</v>
       </c>
     </row>
@@ -1186,24 +1188,24 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11" t="s">
+      <c r="H4" s="13"/>
+      <c r="I4" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -1215,26 +1217,26 @@
       <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11" t="s">
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -1246,28 +1248,28 @@
       <c r="D6" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11" t="s">
+      <c r="H6" s="13"/>
+      <c r="I6" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11" t="s">
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -1279,24 +1281,24 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11" t="s">
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -1308,22 +1310,22 @@
       <c r="D8" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -1335,30 +1337,30 @@
       <c r="D9" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11" t="s">
+      <c r="I9" s="13"/>
+      <c r="J9" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="K9" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11" t="s">
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -1370,24 +1372,24 @@
       <c r="D10" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11" t="s">
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -1399,24 +1401,24 @@
       <c r="D11" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11" t="s">
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -1425,24 +1427,24 @@
       <c r="B12" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11" t="s">
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -1454,24 +1456,24 @@
       <c r="D13" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -1483,24 +1485,24 @@
       <c r="D14" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -1512,47 +1514,47 @@
       <c r="D15" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11" t="s">
+      <c r="H15" s="13"/>
+      <c r="I15" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11" t="s">
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="T15" s="11"/>
+      <c r="T15" s="13"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-      <c r="S16" s="11"/>
-      <c r="T16" s="11"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13"/>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D17" s="14"/>
+      <c r="D17" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1560,7 +1562,7 @@
     <mergeCell ref="G1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup scale="32" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -1606,7 +1608,7 @@
       <c r="E3" t="s">
         <v>126</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="1" t="s">
         <v>127</v>
       </c>
       <c r="G3" t="s">
@@ -1626,486 +1628,486 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="2">
         <v>1</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="2">
         <v>2</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="2">
         <v>3</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="2">
         <v>4</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="2">
         <v>5</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="2">
         <v>6</v>
       </c>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6">
+      <c r="J9" s="2"/>
+      <c r="K9" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="2">
         <v>7</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="J10" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="2">
         <v>8</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="2">
         <v>9</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="2">
         <v>10</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="2">
         <v>11</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="J14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K14" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="2">
         <v>12</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="J15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K15" s="6">
+      <c r="K15" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="2">
         <v>13</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="J16" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K16" s="6">
+      <c r="K16" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2">
         <v>14</v>
       </c>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6">
+      <c r="J17" s="2"/>
+      <c r="K17" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>